<commit_message>
Début reconfiguration du site
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -662,11 +662,11 @@
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.35"/>

</xml_diff>